<commit_message>
add: add MaterialFilter main body code
</commit_message>
<xml_diff>
--- a/data/Inverse_Design.xlsx
+++ b/data/Inverse_Design.xlsx
@@ -1158,25 +1158,25 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="B18" t="n">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="C18" t="n">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="D18" t="n">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="E18" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="F18" t="n">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="G18" t="n">
-        <v>5</v>
+        <v>0.05</v>
       </c>
       <c r="H18" t="n">
         <v>0</v>
@@ -2921,25 +2921,25 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="B61" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="C61" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="D61" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="E61" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="F61" t="n">
-        <v>9</v>
+        <v>0.09</v>
       </c>
       <c r="G61" t="n">
-        <v>4</v>
+        <v>0.04</v>
       </c>
       <c r="H61" t="n">
         <v>0</v>
@@ -4315,19 +4315,19 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
       <c r="B95" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
       <c r="C95" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
       <c r="D95" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
       <c r="E95" t="n">
-        <v>42</v>
+        <v>0.42</v>
       </c>
       <c r="F95" t="n">
         <v>0</v>
@@ -5258,22 +5258,22 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>12</v>
+        <v>0.12</v>
       </c>
       <c r="B118" t="n">
-        <v>16</v>
+        <v>0.16</v>
       </c>
       <c r="C118" t="n">
-        <v>16</v>
+        <v>0.16</v>
       </c>
       <c r="D118" t="n">
-        <v>16</v>
+        <v>0.16</v>
       </c>
       <c r="E118" t="n">
-        <v>29</v>
+        <v>0.29</v>
       </c>
       <c r="F118" t="n">
-        <v>8</v>
+        <v>0.08</v>
       </c>
       <c r="G118" t="n">
         <v>0</v>
@@ -7226,22 +7226,22 @@
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="B166" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="C166" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="D166" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="E166" t="n">
-        <v>22</v>
+        <v>0.22</v>
       </c>
       <c r="F166" t="n">
-        <v>9</v>
+        <v>0.09</v>
       </c>
       <c r="G166" t="n">
         <v>0</v>
@@ -7267,25 +7267,25 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="B167" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="C167" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="D167" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="E167" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="F167" t="n">
-        <v>9</v>
+        <v>0.09</v>
       </c>
       <c r="G167" t="n">
-        <v>4</v>
+        <v>0.04</v>
       </c>
       <c r="H167" t="n">
         <v>0</v>
@@ -7923,22 +7923,22 @@
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
       <c r="B183" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="C183" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="D183" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="E183" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="F183" t="n">
-        <v>9</v>
+        <v>0.09</v>
       </c>
       <c r="G183" t="n">
         <v>0</v>
@@ -8743,25 +8743,25 @@
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="B203" t="n">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="C203" t="n">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="D203" t="n">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="E203" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="F203" t="n">
-        <v>5</v>
+        <v>0.05</v>
       </c>
       <c r="G203" t="n">
-        <v>5</v>
+        <v>0.05</v>
       </c>
       <c r="H203" t="n">
         <v>0</v>
@@ -10670,22 +10670,22 @@
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
       <c r="B250" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="C250" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="D250" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="E250" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="F250" t="n">
-        <v>9</v>
+        <v>0.09</v>
       </c>
       <c r="G250" t="n">
         <v>0</v>
@@ -11285,22 +11285,22 @@
     </row>
     <row r="265">
       <c r="A265" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="B265" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="C265" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="D265" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="E265" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="F265" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="G265" t="n">
         <v>0</v>
@@ -11449,25 +11449,25 @@
     </row>
     <row r="269">
       <c r="A269" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="B269" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="C269" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="D269" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="E269" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="F269" t="n">
-        <v>9</v>
+        <v>0.09</v>
       </c>
       <c r="G269" t="n">
-        <v>4</v>
+        <v>0.04</v>
       </c>
       <c r="H269" t="n">
         <v>0</v>
@@ -12638,22 +12638,22 @@
     </row>
     <row r="298">
       <c r="A298" t="n">
-        <v>12</v>
+        <v>0.12</v>
       </c>
       <c r="B298" t="n">
-        <v>16</v>
+        <v>0.16</v>
       </c>
       <c r="C298" t="n">
-        <v>16</v>
+        <v>0.16</v>
       </c>
       <c r="D298" t="n">
-        <v>16</v>
+        <v>0.16</v>
       </c>
       <c r="E298" t="n">
-        <v>25</v>
+        <v>0.25</v>
       </c>
       <c r="F298" t="n">
-        <v>12</v>
+        <v>0.12</v>
       </c>
       <c r="G298" t="n">
         <v>0</v>
@@ -16492,25 +16492,25 @@
     </row>
     <row r="392">
       <c r="A392" t="n">
-        <v>11</v>
+        <v>0.11</v>
       </c>
       <c r="B392" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="C392" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="D392" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="E392" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="F392" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="G392" t="n">
-        <v>7</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="H392" t="n">
         <v>0</v>
@@ -17148,22 +17148,22 @@
     </row>
     <row r="408">
       <c r="A408" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="B408" t="n">
-        <v>17</v>
+        <v>0.17</v>
       </c>
       <c r="C408" t="n">
-        <v>17</v>
+        <v>0.17</v>
       </c>
       <c r="D408" t="n">
-        <v>17</v>
+        <v>0.17</v>
       </c>
       <c r="E408" t="n">
-        <v>26</v>
+        <v>0.26</v>
       </c>
       <c r="F408" t="n">
-        <v>8</v>
+        <v>0.08</v>
       </c>
       <c r="G408" t="n">
         <v>0</v>
@@ -19649,22 +19649,22 @@
     </row>
     <row r="469">
       <c r="A469" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="B469" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="C469" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="D469" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="E469" t="n">
-        <v>22</v>
+        <v>0.22</v>
       </c>
       <c r="F469" t="n">
-        <v>9</v>
+        <v>0.09</v>
       </c>
       <c r="G469" t="n">
         <v>0</v>
@@ -20387,22 +20387,22 @@
     </row>
     <row r="487">
       <c r="A487" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="B487" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="C487" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="D487" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="E487" t="n">
-        <v>27</v>
+        <v>0.27</v>
       </c>
       <c r="F487" t="n">
-        <v>4</v>
+        <v>0.04</v>
       </c>
       <c r="G487" t="n">
         <v>0</v>
@@ -20428,22 +20428,22 @@
     </row>
     <row r="488">
       <c r="A488" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
       <c r="B488" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="C488" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="D488" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="E488" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="F488" t="n">
-        <v>9</v>
+        <v>0.09</v>
       </c>
       <c r="G488" t="n">
         <v>0</v>
@@ -21043,25 +21043,25 @@
     </row>
     <row r="503">
       <c r="A503" t="n">
-        <v>12</v>
+        <v>0.12</v>
       </c>
       <c r="B503" t="n">
-        <v>16</v>
+        <v>0.16</v>
       </c>
       <c r="C503" t="n">
-        <v>16</v>
+        <v>0.16</v>
       </c>
       <c r="D503" t="n">
-        <v>16</v>
+        <v>0.16</v>
       </c>
       <c r="E503" t="n">
-        <v>16</v>
+        <v>0.16</v>
       </c>
       <c r="F503" t="n">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="G503" t="n">
-        <v>4</v>
+        <v>0.04</v>
       </c>
       <c r="H503" t="n">
         <v>0</v>
@@ -22478,22 +22478,22 @@
     </row>
     <row r="538">
       <c r="A538" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
       <c r="B538" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="C538" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="D538" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="E538" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="F538" t="n">
-        <v>9</v>
+        <v>0.09</v>
       </c>
       <c r="G538" t="n">
         <v>0</v>
@@ -23831,19 +23831,19 @@
     </row>
     <row r="571">
       <c r="A571" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="B571" t="n">
-        <v>17</v>
+        <v>0.17</v>
       </c>
       <c r="C571" t="n">
-        <v>17</v>
+        <v>0.17</v>
       </c>
       <c r="D571" t="n">
-        <v>17</v>
+        <v>0.17</v>
       </c>
       <c r="E571" t="n">
-        <v>34</v>
+        <v>0.34</v>
       </c>
       <c r="F571" t="n">
         <v>0</v>
@@ -23913,22 +23913,22 @@
     </row>
     <row r="573">
       <c r="A573" t="n">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="B573" t="n">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="C573" t="n">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="D573" t="n">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="E573" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="F573" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="G573" t="n">
         <v>0</v>
@@ -24323,25 +24323,25 @@
     </row>
     <row r="583">
       <c r="A583" t="n">
-        <v>11</v>
+        <v>0.11</v>
       </c>
       <c r="B583" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="C583" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="D583" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="E583" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="F583" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="G583" t="n">
-        <v>3</v>
+        <v>0.03</v>
       </c>
       <c r="H583" t="n">
         <v>0</v>
@@ -25020,22 +25020,22 @@
     </row>
     <row r="600">
       <c r="A600" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="B600" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="C600" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="D600" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="E600" t="n">
-        <v>22</v>
+        <v>0.22</v>
       </c>
       <c r="F600" t="n">
-        <v>9</v>
+        <v>0.09</v>
       </c>
       <c r="G600" t="n">
         <v>0</v>
@@ -26455,22 +26455,22 @@
     </row>
     <row r="635">
       <c r="A635" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="B635" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="C635" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="D635" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="E635" t="n">
-        <v>22</v>
+        <v>0.22</v>
       </c>
       <c r="F635" t="n">
-        <v>9</v>
+        <v>0.09</v>
       </c>
       <c r="G635" t="n">
         <v>0</v>
@@ -29243,22 +29243,22 @@
     </row>
     <row r="703">
       <c r="A703" t="n">
-        <v>11</v>
+        <v>0.11</v>
       </c>
       <c r="B703" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="C703" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="D703" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="E703" t="n">
-        <v>23</v>
+        <v>0.23</v>
       </c>
       <c r="F703" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="G703" t="n">
         <v>0</v>
@@ -29776,22 +29776,22 @@
     </row>
     <row r="716">
       <c r="A716" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="B716" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="C716" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="D716" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="E716" t="n">
-        <v>22</v>
+        <v>0.22</v>
       </c>
       <c r="F716" t="n">
-        <v>9</v>
+        <v>0.09</v>
       </c>
       <c r="G716" t="n">
         <v>0</v>
@@ -30801,22 +30801,22 @@
     </row>
     <row r="741">
       <c r="A741" t="n">
-        <v>12</v>
+        <v>0.12</v>
       </c>
       <c r="B741" t="n">
-        <v>16</v>
+        <v>0.16</v>
       </c>
       <c r="C741" t="n">
-        <v>16</v>
+        <v>0.16</v>
       </c>
       <c r="D741" t="n">
-        <v>16</v>
+        <v>0.16</v>
       </c>
       <c r="E741" t="n">
-        <v>24</v>
+        <v>0.24</v>
       </c>
       <c r="F741" t="n">
-        <v>16</v>
+        <v>0.16</v>
       </c>
       <c r="G741" t="n">
         <v>0</v>
@@ -32359,22 +32359,22 @@
     </row>
     <row r="779">
       <c r="A779" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
       <c r="B779" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="C779" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="D779" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="E779" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="F779" t="n">
-        <v>9</v>
+        <v>0.09</v>
       </c>
       <c r="G779" t="n">
         <v>0</v>
@@ -33179,22 +33179,22 @@
     </row>
     <row r="799">
       <c r="A799" t="n">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="B799" t="n">
-        <v>21</v>
+        <v>0.21</v>
       </c>
       <c r="C799" t="n">
-        <v>21</v>
+        <v>0.21</v>
       </c>
       <c r="D799" t="n">
-        <v>21</v>
+        <v>0.21</v>
       </c>
       <c r="E799" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="F799" t="n">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="G799" t="n">
         <v>0</v>
@@ -34983,25 +34983,25 @@
     </row>
     <row r="843">
       <c r="A843" t="n">
-        <v>11</v>
+        <v>0.11</v>
       </c>
       <c r="B843" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="C843" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="D843" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="E843" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="F843" t="n">
-        <v>23</v>
+        <v>0.23</v>
       </c>
       <c r="G843" t="n">
-        <v>3</v>
+        <v>0.03</v>
       </c>
       <c r="H843" t="n">
         <v>0</v>
@@ -36828,22 +36828,22 @@
     </row>
     <row r="888">
       <c r="A888" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
       <c r="B888" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="C888" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="D888" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="E888" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="F888" t="n">
-        <v>9</v>
+        <v>0.09</v>
       </c>
       <c r="G888" t="n">
         <v>0</v>
@@ -37402,19 +37402,19 @@
     </row>
     <row r="902">
       <c r="A902" t="n">
-        <v>14</v>
+        <v>0.14</v>
       </c>
       <c r="B902" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="C902" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="D902" t="n">
-        <v>19</v>
+        <v>0.19</v>
       </c>
       <c r="E902" t="n">
-        <v>28</v>
+        <v>0.28</v>
       </c>
       <c r="F902" t="n">
         <v>0</v>
@@ -40231,19 +40231,19 @@
     </row>
     <row r="971">
       <c r="A971" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="B971" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="C971" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="D971" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="E971" t="n">
-        <v>46</v>
+        <v>0.46</v>
       </c>
       <c r="F971" t="n">
         <v>0</v>
@@ -40313,19 +40313,19 @@
     </row>
     <row r="973">
       <c r="A973" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="B973" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="C973" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="D973" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="E973" t="n">
-        <v>31</v>
+        <v>0.31</v>
       </c>
       <c r="F973" t="n">
         <v>0</v>
@@ -41871,25 +41871,25 @@
     </row>
     <row r="1011">
       <c r="A1011" t="n">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="B1011" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="C1011" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="D1011" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="E1011" t="n">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="F1011" t="n">
-        <v>9</v>
+        <v>0.09</v>
       </c>
       <c r="G1011" t="n">
-        <v>4</v>
+        <v>0.04</v>
       </c>
       <c r="H1011" t="n">
         <v>0</v>
@@ -42076,25 +42076,25 @@
     </row>
     <row r="1016">
       <c r="A1016" t="n">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="B1016" t="n">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="C1016" t="n">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="D1016" t="n">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="E1016" t="n">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="F1016" t="n">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="G1016" t="n">
-        <v>5</v>
+        <v>0.05</v>
       </c>
       <c r="H1016" t="n">
         <v>0</v>

</xml_diff>